<commit_message>
feat: added a validator to resultTracker
</commit_message>
<xml_diff>
--- a/src/main/resources/analytics/ResultTracker.xlsx
+++ b/src/main/resources/analytics/ResultTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/achan625_uwo_ca/Documents/Coding/BlackjackSimulator/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\IdeaProjects\BlackjackSimulator\src\main\resources\analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{0AF35517-C79C-4059-AFB4-5399EA0E15D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB9C7865-DC88-4B82-B0C4-18687EA2BECF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD049250-BB7F-4698-9728-E4C73A6557D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Round</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Loss %</t>
+  </si>
+  <si>
+    <t>Expected Payout</t>
+  </si>
+  <si>
+    <t>Validator</t>
   </si>
 </sst>
 </file>
@@ -164,10 +170,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -486,17 +488,19 @@
     <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.21875" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.21875" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,147 +531,161 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L2" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <f>$O$1*SUM(C2*1.5,D2,E2*2,-G2*2,-H2,-I2*2,-J2)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(K2+B2=B3,"","XXXX")</f>
+        <v/>
+      </c>
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1">
-        <f>$M$1*(SUM(C:J)+SUM(E:E,G:G,I:I))</f>
+      <c r="O2" s="1">
+        <f>$O$1*(SUM(C:J)+SUM(E:E,G:G,I:I))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L3" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="1">
-        <f>$M$1*(SUM(D:D)+2*SUM(E:E)+1.5*SUM(C:C))</f>
+      <c r="O3" s="1">
+        <f>$O$1*(SUM(D:D)+2*SUM(E:E)+1.5*SUM(C:C))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L4" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="1">
-        <f>$M$1*(SUM(J:J,H:H)+2*SUM(I:I,G:G))</f>
+      <c r="O4" s="1">
+        <f>$O$1*(SUM(J:J,H:H)+2*SUM(I:I,G:G))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L5" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="2">
-        <f>M4-M3</f>
+      <c r="O5" s="2">
+        <f>O4-O3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L6" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="3" t="e">
-        <f>M5/M2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L8" t="str">
+      <c r="O6" s="3" t="e">
+        <f>O5/O2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N8" t="str">
         <f>_xlfn.CONCAT(C1, " %")</f>
         <v>BLACKJACK %</v>
       </c>
-      <c r="M8" t="str">
-        <f t="shared" ref="M8:S8" si="0">_xlfn.CONCAT(D1, " %")</f>
+      <c r="O8" t="str">
+        <f>_xlfn.CONCAT(D1, " %")</f>
         <v>WIN %</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" t="str">
+        <f>_xlfn.CONCAT(E1, " %")</f>
+        <v>DOUBLE_WIN %</v>
+      </c>
+      <c r="Q8" t="str">
+        <f>_xlfn.CONCAT(F1, " %")</f>
+        <v>PUSH %</v>
+      </c>
+      <c r="R8" t="str">
+        <f>_xlfn.CONCAT(G1, " %")</f>
+        <v>DOUBLE_BUST %</v>
+      </c>
+      <c r="S8" t="str">
+        <f>_xlfn.CONCAT(H1, " %")</f>
+        <v>BUST %</v>
+      </c>
+      <c r="T8" t="str">
+        <f>_xlfn.CONCAT(I1, " %")</f>
+        <v>DOUBLE_LOSE %</v>
+      </c>
+      <c r="U8" t="str">
+        <f>_xlfn.CONCAT(J1, " %")</f>
+        <v>LOSE %</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N9" s="5" t="e">
+        <f>SUM(C:C)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="5" t="e">
+        <f t="shared" ref="O9:U9" si="0">SUM(D:D)/SUM($C:$J)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>DOUBLE_WIN %</v>
-      </c>
-      <c r="O8" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>PUSH %</v>
-      </c>
-      <c r="P8" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>DOUBLE_BUST %</v>
-      </c>
-      <c r="Q8" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>BUST %</v>
-      </c>
-      <c r="R8" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>DOUBLE_LOSE %</v>
-      </c>
-      <c r="S8" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="5" t="e">
         <f t="shared" si="0"/>
-        <v>LOSE %</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L9" s="5" t="e">
-        <f>SUM(C:C)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="5" t="e">
-        <f t="shared" ref="M9:S9" si="1">SUM(D:D)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L11" t="s">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" s="3"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="4" t="e">
+      <c r="O11" s="4" t="e">
         <f>SUM(C:E)/SUM($C:$J)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L12" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="4" t="e">
+      <c r="O12" s="4" t="e">
         <f>SUM(F:F)/SUM($C:$J)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="L13" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="4" t="e">
+      <c r="O13" s="4" t="e">
         <f>SUM(G:J)/SUM(C:J)</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
feat: track diff bets and refactored edge calc
</commit_message>
<xml_diff>
--- a/src/main/resources/analytics/ResultTracker.xlsx
+++ b/src/main/resources/analytics/ResultTracker.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\IdeaProjects\BlackjackSimulator\src\main\resources\analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\BlackjackSimulator\src\main\resources\analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD049250-BB7F-4698-9728-E4C73A6557D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCF87A1-62D0-4213-B2D9-7EA4F0374EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Round</t>
   </si>
@@ -65,15 +65,9 @@
     <t>LOSE</t>
   </si>
   <si>
-    <t>Total Amount Bet</t>
-  </si>
-  <si>
     <t>House Edge</t>
   </si>
   <si>
-    <t>Bet Size</t>
-  </si>
-  <si>
     <t>Total Won</t>
   </si>
   <si>
@@ -92,10 +86,22 @@
     <t>Loss %</t>
   </si>
   <si>
-    <t>Expected Payout</t>
-  </si>
-  <si>
-    <t>Validator</t>
+    <t>Initial Bet</t>
+  </si>
+  <si>
+    <t>Amount Won</t>
+  </si>
+  <si>
+    <t>Amount Lost</t>
+  </si>
+  <si>
+    <t>Amount Wagered</t>
+  </si>
+  <si>
+    <t>Total Amount Wagered</t>
+  </si>
+  <si>
+    <t>Minimum Bet Size</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -480,27 +486,30 @@
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" customWidth="1"/>
-    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.21875" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.21875" customWidth="1"/>
+    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,185 +517,195 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>C2*SUM(D2*1.5,E2,2*F2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>C2*SUM(I2,K2,2*H2,2*J2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>C2*(SUM(D2:K2)+SUM(F2,H2,J2))</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(N:N)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>SUM(L:L)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="K2">
-        <f>$O$1*SUM(C2*1.5,D2,E2*2,-G2*2,-H2,-I2*2,-J2)</f>
+      <c r="Q4" s="1">
+        <f>SUM(M:M)</f>
         <v>0</v>
       </c>
-      <c r="L2" t="str">
-        <f>IF(K2+B2=B3,"","XXXX")</f>
-        <v/>
-      </c>
-      <c r="N2" t="s">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>Q4-Q3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="1">
-        <f>$O$1*(SUM(C:J)+SUM(E:E,G:G,I:I))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="1">
-        <f>$O$1*(SUM(D:D)+2*SUM(E:E)+1.5*SUM(C:C))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N4" t="s">
+      <c r="Q6" s="3" t="e">
+        <f>Q5/Q2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P8" t="str">
+        <f t="shared" ref="P8:W8" si="0">_xlfn.CONCAT(D1, " %")</f>
+        <v>BLACKJACK %</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v>WIN %</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_WIN %</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>PUSH %</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_BUST %</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="0"/>
+        <v>BUST %</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="0"/>
+        <v>DOUBLE_LOSE %</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="0"/>
+        <v>LOSE %</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P9" s="5" t="e">
+        <f>SUM(D:D)/SUM($D:$K)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="5" t="e">
+        <f t="shared" ref="Q9:W9" si="1">SUM(E:E)/SUM($D:$K)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W9" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X9" s="3"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="1">
-        <f>$O$1*(SUM(J:J,H:H)+2*SUM(I:I,G:G))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N5" t="s">
+      <c r="Q11" s="4" t="e">
+        <f>SUM(D:F)/SUM($D:$K)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P12" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="2">
-        <f>O4-O3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O6" s="3" t="e">
-        <f>O5/O2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N8" t="str">
-        <f>_xlfn.CONCAT(C1, " %")</f>
-        <v>BLACKJACK %</v>
-      </c>
-      <c r="O8" t="str">
-        <f>_xlfn.CONCAT(D1, " %")</f>
-        <v>WIN %</v>
-      </c>
-      <c r="P8" t="str">
-        <f>_xlfn.CONCAT(E1, " %")</f>
-        <v>DOUBLE_WIN %</v>
-      </c>
-      <c r="Q8" t="str">
-        <f>_xlfn.CONCAT(F1, " %")</f>
-        <v>PUSH %</v>
-      </c>
-      <c r="R8" t="str">
-        <f>_xlfn.CONCAT(G1, " %")</f>
-        <v>DOUBLE_BUST %</v>
-      </c>
-      <c r="S8" t="str">
-        <f>_xlfn.CONCAT(H1, " %")</f>
-        <v>BUST %</v>
-      </c>
-      <c r="T8" t="str">
-        <f>_xlfn.CONCAT(I1, " %")</f>
-        <v>DOUBLE_LOSE %</v>
-      </c>
-      <c r="U8" t="str">
-        <f>_xlfn.CONCAT(J1, " %")</f>
-        <v>LOSE %</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N9" s="5" t="e">
-        <f>SUM(C:C)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="5" t="e">
-        <f t="shared" ref="O9:U9" si="0">SUM(D:D)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U9" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V9" s="3"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N11" t="s">
+      <c r="Q12" s="4" t="e">
+        <f>SUM(G:G)/SUM($D:$K)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="4" t="e">
-        <f>SUM(C:E)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N12" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" s="4" t="e">
-        <f>SUM(F:F)/SUM($C:$J)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" s="4" t="e">
-        <f>SUM(G:J)/SUM(C:J)</f>
+      <c r="Q13" s="4" t="e">
+        <f>SUM(H:K)/SUM(D:K)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>